<commit_message>
added Area.fromChunkIndex() + implemented chunks in Grid.devFill()
</commit_message>
<xml_diff>
--- a/dev/GridPositioning.xlsx
+++ b/dev/GridPositioning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fes\Desktop\Code\Townly\engine\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E5D70B6-3B55-4613-B519-D581959F7EE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C94714-1873-4E07-B90D-C9AAA2D5C468}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8C409D7-9037-44E1-BE6F-DEDA12A1AF10}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Abs: 28,20</t>
   </si>
@@ -71,6 +71,24 @@
   <si>
     <t>Rel: 0,9</t>
   </si>
+  <si>
+    <t>Rel = Position relative to Chunk</t>
+  </si>
+  <si>
+    <t>CIDX = Chunk Index relative to Grid</t>
+  </si>
+  <si>
+    <t>Abs = Position absolute to Grid</t>
+  </si>
+  <si>
+    <t>Note: Excel columns and rows start</t>
+  </si>
+  <si>
+    <t>at 1, Teng positions however start</t>
+  </si>
+  <si>
+    <t>at 0, so subtract 1 to get the Teng pos</t>
+  </si>
 </sst>
 </file>
 
@@ -92,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +159,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -182,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -199,6 +229,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -516,7 +548,7 @@
   <dimension ref="A1:BG103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF11" sqref="AF11"/>
+      <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +556,10 @@
     <col min="1" max="20" width="2.7109375" customWidth="1"/>
     <col min="21" max="30" width="2.7109375" style="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="7" customWidth="1"/>
-    <col min="32" max="59" width="11.42578125" style="7"/>
+    <col min="32" max="32" width="10.7109375" style="7" customWidth="1"/>
+    <col min="33" max="33" width="4.7109375" style="7" customWidth="1"/>
+    <col min="34" max="34" width="35" style="7" customWidth="1"/>
+    <col min="35" max="59" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -1048,7 +1083,7 @@
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1080,7 +1115,7 @@
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1115,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1150,7 +1185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1185,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1217,7 +1252,7 @@
       <c r="AC21" s="9"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1249,7 +1284,7 @@
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1283,8 +1318,11 @@
       <c r="AF23" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH23" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1318,8 +1356,11 @@
       <c r="AF24" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH24" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1353,8 +1394,11 @@
       <c r="AF25" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH25" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1386,7 +1430,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1418,7 +1462,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1452,8 +1496,11 @@
       <c r="AF28" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH28" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1487,8 +1534,11 @@
       <c r="AF29" s="14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH29" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1522,8 +1572,11 @@
       <c r="AF30" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH30" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1555,7 +1608,7 @@
       <c r="AC31" s="8"/>
       <c r="AD31" s="8"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>

</xml_diff>

<commit_message>
accidentally changed grid positioning spreadsheet
</commit_message>
<xml_diff>
--- a/dev/GridPositioning.xlsx
+++ b/dev/GridPositioning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fes\Desktop\Code\Townly\engine\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C94714-1873-4E07-B90D-C9AAA2D5C468}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B67CFA-689F-41CA-862B-04F6004401D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8C409D7-9037-44E1-BE6F-DEDA12A1AF10}"/>
+    <workbookView xWindow="28680" yWindow="-11865" windowWidth="29040" windowHeight="15840" xr2:uid="{F8C409D7-9037-44E1-BE6F-DEDA12A1AF10}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -548,7 +548,7 @@
   <dimension ref="A1:BG103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>